<commit_message>
417: Configure for Auzre SQL
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/WMT_Extract_sample.xlsx
+++ b/wmt_etl/tests/data/WMT_Extract_sample.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomassw/SOURCE/kainos/NOMS/WMT/wmt-etl/wmt_etl/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomassw/SOURCE/kainos/NOMS/WMT/wmt-etl/wmt_etl/tests/data/full_inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="31360" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="79">
   <si>
     <t>Trust</t>
   </si>
@@ -101,30 +101,6 @@
     <t>CommTierA</t>
   </si>
   <si>
-    <t>LicenseTier0</t>
-  </si>
-  <si>
-    <t>LicenseTierD2</t>
-  </si>
-  <si>
-    <t>LicenseTierD1</t>
-  </si>
-  <si>
-    <t>LicenseTierC2</t>
-  </si>
-  <si>
-    <t>LicenseTierC1</t>
-  </si>
-  <si>
-    <t>LicenseTierB2</t>
-  </si>
-  <si>
-    <t>LicenseTierB1</t>
-  </si>
-  <si>
-    <t>LicenseTierA</t>
-  </si>
-  <si>
     <t>CustTier0</t>
   </si>
   <si>
@@ -164,9 +140,6 @@
     <t>London</t>
   </si>
   <si>
-    <t>LDN</t>
-  </si>
-  <si>
     <t>KainosLDU</t>
   </si>
   <si>
@@ -225,13 +198,85 @@
   </si>
   <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>OM_Name</t>
+  </si>
+  <si>
+    <t>Parom_Comp_Last_30</t>
+  </si>
+  <si>
+    <t>Parom_Due_Next_30</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Community</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>NPSQ</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>X555555</t>
+  </si>
+  <si>
+    <t>X444444</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>1001</t>
+  </si>
+  <si>
+    <t>1002</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>ND01</t>
+  </si>
+  <si>
+    <t>LicenceTier0</t>
+  </si>
+  <si>
+    <t>LicenceTierD2</t>
+  </si>
+  <si>
+    <t>LicenceTierD1</t>
+  </si>
+  <si>
+    <t>LicenceTierC2</t>
+  </si>
+  <si>
+    <t>LicenceTierC1</t>
+  </si>
+  <si>
+    <t>LicenceTierB2</t>
+  </si>
+  <si>
+    <t>LicenceTierB1</t>
+  </si>
+  <si>
+    <t>LicenceTierA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -249,16 +294,43 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -266,17 +338,85 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCAC9D9"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCAC9D9"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCAC9D9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCAC9D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFCAC9D9"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCAC9D9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCAC9D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCAC9D9"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCAC9D9"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFCAC9D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFCAC9D9"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFCAC9D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -554,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AO1" sqref="AO1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -658,93 +798,93 @@
         <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AF1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AI1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AN1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AO1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" t="s">
         <v>41</v>
-      </c>
-      <c r="B2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" t="s">
-        <v>50</v>
       </c>
       <c r="K2">
         <v>1001</v>
@@ -842,34 +982,34 @@
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
         <v>42</v>
       </c>
-      <c r="C3" t="s">
+      <c r="I3" t="s">
         <v>43</v>
       </c>
-      <c r="D3" t="s">
+      <c r="J3" t="s">
         <v>44</v>
-      </c>
-      <c r="E3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I3" t="s">
-        <v>52</v>
-      </c>
-      <c r="J3" t="s">
-        <v>53</v>
       </c>
       <c r="K3">
         <v>1002</v>
@@ -972,60 +1112,104 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>55</v>
       </c>
-      <c r="C1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2">
+        <v>1001</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2">
         <v>15</v>
       </c>
-      <c r="C2">
+      <c r="G2">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="H2">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="I2" s="3">
+        <v>42795.628472222219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3">
+        <v>1002</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3">
         <v>18</v>
       </c>
-      <c r="C3">
+      <c r="G3">
         <v>11</v>
       </c>
-      <c r="D3">
+      <c r="H3">
         <v>13</v>
+      </c>
+      <c r="I3" s="3">
+        <v>42795.628472222219</v>
       </c>
     </row>
   </sheetData>
@@ -1035,10 +1219,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1047,48 +1231,85 @@
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>55</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2">
-        <v>15</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
       </c>
       <c r="D2">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1001</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="H2" s="3">
+        <v>42795.628472222219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3">
-        <v>18</v>
-      </c>
-      <c r="C3">
-        <v>11</v>
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
       </c>
       <c r="D3">
-        <v>13</v>
+        <v>1002</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3">
+        <v>42795.628472222219</v>
       </c>
     </row>
   </sheetData>
@@ -1098,23 +1319,32 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="A2" sqref="A2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -1126,7 +1356,53 @@
         <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>63</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1136,23 +1412,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -1164,7 +1440,53 @@
         <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>63</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1174,23 +1496,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -1202,7 +1524,53 @@
         <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>63</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1212,23 +1580,23 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -1240,7 +1608,53 @@
         <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>63</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
989: Fixes for unit and integration tests
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/WMT_Extract_sample.xlsx
+++ b/wmt_etl/tests/data/WMT_Extract_sample.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomassw/SOURCE/kainos/NOMS/WMT/wmt-etl/wmt_etl/tests/data/full_inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/terences/Sources/WMT/wmt-etl/wmt_etl/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Flag_Upw" sheetId="5" r:id="rId5"/>
     <sheet name="Flag_O_Due" sheetId="6" r:id="rId6"/>
     <sheet name="Flag_Priority" sheetId="7" r:id="rId7"/>
+    <sheet name="CMS" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="100">
   <si>
     <t>Trust</t>
   </si>
@@ -270,13 +271,83 @@
   </si>
   <si>
     <t>LicenceTierA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact_ID
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact_Date
+</t>
+  </si>
+  <si>
+    <t>Contact_Type_Code</t>
+  </si>
+  <si>
+    <t>Contact_Type_Desc</t>
+  </si>
+  <si>
+    <t>Contact_Staff_Name</t>
+  </si>
+  <si>
+    <t>Contact_Staff_Key</t>
+  </si>
+  <si>
+    <t>Contact_Staff_Grade</t>
+  </si>
+  <si>
+    <t>Contact_Team_Key</t>
+  </si>
+  <si>
+    <t>Contact_Provider_Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OM_Name
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OM_Key
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OM_Grade
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OM_Team_Key
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OM_Provider_Code
+</t>
+  </si>
+  <si>
+    <t>CMS1</t>
+  </si>
+  <si>
+    <t>The first type</t>
+  </si>
+  <si>
+    <t>Andy Wright</t>
+  </si>
+  <si>
+    <t>Tom Swann</t>
+  </si>
+  <si>
+    <t>CMS2</t>
+  </si>
+  <si>
+    <t>The second type</t>
+  </si>
+  <si>
+    <t>Any Wright</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -314,6 +385,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -396,7 +472,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -413,6 +489,13 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -694,7 +777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
@@ -1660,4 +1743,151 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" s="8" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="9">
+        <v>123</v>
+      </c>
+      <c r="B2" s="10">
+        <v>42991</v>
+      </c>
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2">
+        <v>1002</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K2">
+        <v>1001</v>
+      </c>
+      <c r="L2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>321</v>
+      </c>
+      <c r="B3" s="10">
+        <v>42991</v>
+      </c>
+      <c r="C3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3">
+        <v>1001</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" t="s">
+        <v>99</v>
+      </c>
+      <c r="K3">
+        <v>1002</v>
+      </c>
+      <c r="L3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
989: Adds CMS to test imports and cms table to extract process (#13)
* 989: Adds CMS to test imports and cms table to extract process

* 989: Fixes for unit and integration tests

* 989: formatting fix

* 989: updates test data to include thrid cms reason

* 989: changes to make new team in ND02 file
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/WMT_Extract_sample.xlsx
+++ b/wmt_etl/tests/data/WMT_Extract_sample.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomassw/SOURCE/kainos/NOMS/WMT/wmt-etl/wmt_etl/tests/data/full_inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/terences/Sources/WMT/wmt-etl/wmt_etl/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Flag_Upw" sheetId="5" r:id="rId5"/>
     <sheet name="Flag_O_Due" sheetId="6" r:id="rId6"/>
     <sheet name="Flag_Priority" sheetId="7" r:id="rId7"/>
+    <sheet name="CMS" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="100">
   <si>
     <t>Trust</t>
   </si>
@@ -270,13 +271,83 @@
   </si>
   <si>
     <t>LicenceTierA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact_ID
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact_Date
+</t>
+  </si>
+  <si>
+    <t>Contact_Type_Code</t>
+  </si>
+  <si>
+    <t>Contact_Type_Desc</t>
+  </si>
+  <si>
+    <t>Contact_Staff_Name</t>
+  </si>
+  <si>
+    <t>Contact_Staff_Key</t>
+  </si>
+  <si>
+    <t>Contact_Staff_Grade</t>
+  </si>
+  <si>
+    <t>Contact_Team_Key</t>
+  </si>
+  <si>
+    <t>Contact_Provider_Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OM_Name
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OM_Key
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OM_Grade
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OM_Team_Key
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OM_Provider_Code
+</t>
+  </si>
+  <si>
+    <t>CMS1</t>
+  </si>
+  <si>
+    <t>The first type</t>
+  </si>
+  <si>
+    <t>Andy Wright</t>
+  </si>
+  <si>
+    <t>Tom Swann</t>
+  </si>
+  <si>
+    <t>CMS2</t>
+  </si>
+  <si>
+    <t>The second type</t>
+  </si>
+  <si>
+    <t>Any Wright</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -314,6 +385,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -396,7 +472,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -413,6 +489,13 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -694,7 +777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
@@ -1660,4 +1743,151 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" s="8" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="9">
+        <v>123</v>
+      </c>
+      <c r="B2" s="10">
+        <v>42991</v>
+      </c>
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2">
+        <v>1002</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K2">
+        <v>1001</v>
+      </c>
+      <c r="L2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>321</v>
+      </c>
+      <c r="B3" s="10">
+        <v>42991</v>
+      </c>
+      <c r="C3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3">
+        <v>1001</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" t="s">
+        <v>99</v>
+      </c>
+      <c r="K3">
+        <v>1002</v>
+      </c>
+      <c r="L3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
977: Add GS to extract process and GS tab to example files
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/WMT_Extract_sample.xlsx
+++ b/wmt_etl/tests/data/WMT_Extract_sample.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/terences/Sources/WMT/wmt-etl/wmt_etl/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caoimheb/Documents/MOJ_WMT/repos/wmt-etl/wmt_etl/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Flag_O_Due" sheetId="6" r:id="rId6"/>
     <sheet name="Flag_Priority" sheetId="7" r:id="rId7"/>
     <sheet name="CMS" sheetId="8" r:id="rId8"/>
+    <sheet name="GS" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="105">
   <si>
     <t>Trust</t>
   </si>
@@ -341,13 +342,28 @@
   </si>
   <si>
     <t>Any Wright</t>
+  </si>
+  <si>
+    <t>Contact_ID</t>
+  </si>
+  <si>
+    <t>Contact_Date</t>
+  </si>
+  <si>
+    <t>OM_Grade</t>
+  </si>
+  <si>
+    <t>OM_Team_Key</t>
+  </si>
+  <si>
+    <t>OM_Provider_Code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -390,6 +406,13 @@
       <sz val="9"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -472,7 +495,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -496,6 +519,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1749,7 +1773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -1890,4 +1914,48 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
996: Add T2A to xlsx files and extract process
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/WMT_Extract_sample.xlsx
+++ b/wmt_etl/tests/data/WMT_Extract_sample.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Flag_Priority" sheetId="7" r:id="rId7"/>
     <sheet name="CMS" sheetId="8" r:id="rId8"/>
     <sheet name="GS" sheetId="9" r:id="rId9"/>
+    <sheet name="T2A" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="105">
   <si>
     <t>Trust</t>
   </si>
@@ -802,7 +803,7 @@
   <dimension ref="A1:AO3"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2"/>
+      <selection activeCell="D1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1217,6 +1218,146 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AO1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:41" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
@@ -1920,7 +2061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
414: Update sample file used for testing
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/WMT_Extract_sample.xlsx
+++ b/wmt_etl/tests/data/WMT_Extract_sample.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/terences/Sources/WMT/wmt-etl/wmt_etl/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewwr/src/wmt/etl/wmt_etl/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Flag_O_Due" sheetId="6" r:id="rId6"/>
     <sheet name="Flag_Priority" sheetId="7" r:id="rId7"/>
     <sheet name="CMS" sheetId="8" r:id="rId8"/>
+    <sheet name="ARMS" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="119">
   <si>
     <t>Trust</t>
   </si>
@@ -341,13 +342,70 @@
   </si>
   <si>
     <t>Any Wright</t>
+  </si>
+  <si>
+    <t>Assessment_Date</t>
+  </si>
+  <si>
+    <t>Assessment_Code</t>
+  </si>
+  <si>
+    <t>Assessment_Desc</t>
+  </si>
+  <si>
+    <t>Assessment_Staff_Name</t>
+  </si>
+  <si>
+    <t>Assessment_Staff_Key</t>
+  </si>
+  <si>
+    <t>Assessment_Staff_Grade</t>
+  </si>
+  <si>
+    <t>Assessmentent_Team_Key</t>
+  </si>
+  <si>
+    <t>Assessment_Provider_Code</t>
+  </si>
+  <si>
+    <t>CRN</t>
+  </si>
+  <si>
+    <t>Disposal_or_Release_Date</t>
+  </si>
+  <si>
+    <t>Sentence_Type</t>
+  </si>
+  <si>
+    <t>SO_Registration_Date</t>
+  </si>
+  <si>
+    <t>ARMS1</t>
+  </si>
+  <si>
+    <t>Test Arms Assessment</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>C1234567</t>
+  </si>
+  <si>
+    <t>License</t>
+  </si>
+  <si>
+    <t>C1234568</t>
+  </si>
+  <si>
+    <t>ARMS2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -391,8 +449,21 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -405,8 +476,20 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0B64A0"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8FBFC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -466,13 +549,102 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3877A6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3877A6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3877A6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA5A5B1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3877A6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3877A6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA5A5B1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3877A6"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFEBEBEB"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFEBEBEB"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFEBEBEB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFEBEBEB"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFEBEBEB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFEBEBEB"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFEBEBEB"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFEBEBEB"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -496,6 +668,35 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1749,7 +1950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -1890,4 +2091,137 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="37" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="16">
+        <v>42991</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="19">
+        <v>1002</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="J2" s="16">
+        <v>42991</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="L2" s="16">
+        <v>42991</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="16">
+        <v>42991</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="19">
+        <v>1002</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="J3" s="16">
+        <v>42991</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" s="16">
+        <v>42991</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Feature/wmt 414/display arms assessments (#15)
* 414: Add ARMS tab to test extract files

* 414: Update ELT to handle ARMS tab

* 414: Rename `sentence type` to `sentence_type`

We will need to ensure that this is what it will be called in the actual
extract.

* 414: Update sample file used for testing
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/WMT_Extract_sample.xlsx
+++ b/wmt_etl/tests/data/WMT_Extract_sample.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/terences/Sources/WMT/wmt-etl/wmt_etl/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewwr/src/wmt/etl/wmt_etl/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Flag_O_Due" sheetId="6" r:id="rId6"/>
     <sheet name="Flag_Priority" sheetId="7" r:id="rId7"/>
     <sheet name="CMS" sheetId="8" r:id="rId8"/>
+    <sheet name="ARMS" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="119">
   <si>
     <t>Trust</t>
   </si>
@@ -341,13 +342,70 @@
   </si>
   <si>
     <t>Any Wright</t>
+  </si>
+  <si>
+    <t>Assessment_Date</t>
+  </si>
+  <si>
+    <t>Assessment_Code</t>
+  </si>
+  <si>
+    <t>Assessment_Desc</t>
+  </si>
+  <si>
+    <t>Assessment_Staff_Name</t>
+  </si>
+  <si>
+    <t>Assessment_Staff_Key</t>
+  </si>
+  <si>
+    <t>Assessment_Staff_Grade</t>
+  </si>
+  <si>
+    <t>Assessmentent_Team_Key</t>
+  </si>
+  <si>
+    <t>Assessment_Provider_Code</t>
+  </si>
+  <si>
+    <t>CRN</t>
+  </si>
+  <si>
+    <t>Disposal_or_Release_Date</t>
+  </si>
+  <si>
+    <t>Sentence_Type</t>
+  </si>
+  <si>
+    <t>SO_Registration_Date</t>
+  </si>
+  <si>
+    <t>ARMS1</t>
+  </si>
+  <si>
+    <t>Test Arms Assessment</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>C1234567</t>
+  </si>
+  <si>
+    <t>License</t>
+  </si>
+  <si>
+    <t>C1234568</t>
+  </si>
+  <si>
+    <t>ARMS2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -391,8 +449,21 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -405,8 +476,20 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0B64A0"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8FBFC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -466,13 +549,102 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3877A6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3877A6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3877A6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA5A5B1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3877A6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3877A6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA5A5B1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3877A6"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFEBEBEB"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFEBEBEB"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFEBEBEB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFEBEBEB"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFEBEBEB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFEBEBEB"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFEBEBEB"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFEBEBEB"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -496,6 +668,35 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1749,7 +1950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -1890,4 +2091,137 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="37" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="16">
+        <v>42991</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="19">
+        <v>1002</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="J2" s="16">
+        <v>42991</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="L2" s="16">
+        <v>42991</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="16">
+        <v>42991</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="19">
+        <v>1002</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="J3" s="16">
+        <v>42991</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" s="16">
+        <v>42991</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add GS to extract sample
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/WMT_Extract_sample.xlsx
+++ b/wmt_etl/tests/data/WMT_Extract_sample.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="130">
   <si>
     <t>Trust</t>
   </si>
@@ -415,6 +415,24 @@
   </si>
   <si>
     <t>C1234568</t>
+  </si>
+  <si>
+    <t>GS1</t>
+  </si>
+  <si>
+    <t>Group supervision</t>
+  </si>
+  <si>
+    <t>Billy Jones</t>
+  </si>
+  <si>
+    <t>PO</t>
+  </si>
+  <si>
+    <t>JWMT</t>
+  </si>
+  <si>
+    <t>Jane Jones</t>
   </si>
 </sst>
 </file>
@@ -1414,7 +1432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:L3"/>
     </sheetView>
   </sheetViews>
@@ -2240,13 +2258,17 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="22.1640625" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
@@ -2277,6 +2299,64 @@
         <v>104</v>
       </c>
     </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="11">
+        <v>999</v>
+      </c>
+      <c r="B2" s="17">
+        <v>43033</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="11">
+        <v>1003</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="11">
+        <v>888</v>
+      </c>
+      <c r="B3" s="17">
+        <v>43033</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" s="11">
+        <v>1003</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
996: Merge extract file
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/WMT_Extract_sample.xlsx
+++ b/wmt_etl/tests/data/WMT_Extract_sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caoimheb/Documents/MOJ_WMT/repos/wmt-etl/wmt_etl/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caoimheb/Desktop/Excel files /"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,8 @@
     <sheet name="Flag_Priority" sheetId="7" r:id="rId7"/>
     <sheet name="CMS" sheetId="8" r:id="rId8"/>
     <sheet name="GS" sheetId="9" r:id="rId9"/>
-    <sheet name="T2A" sheetId="10" r:id="rId10"/>
+    <sheet name="T2A" sheetId="11" r:id="rId10"/>
+    <sheet name="ARMS" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="130">
   <si>
     <t>Trust</t>
   </si>
@@ -358,13 +359,88 @@
   </si>
   <si>
     <t>OM_Provider_Code</t>
+  </si>
+  <si>
+    <t>Assessment_Date</t>
+  </si>
+  <si>
+    <t>Assessment_Code</t>
+  </si>
+  <si>
+    <t>Assessment_Desc</t>
+  </si>
+  <si>
+    <t>Assessment_Staff_Name</t>
+  </si>
+  <si>
+    <t>Assessment_Staff_Key</t>
+  </si>
+  <si>
+    <t>Assessment_Staff_Grade</t>
+  </si>
+  <si>
+    <t>Assessmentent_Team_Key</t>
+  </si>
+  <si>
+    <t>Assessment_Provider_Code</t>
+  </si>
+  <si>
+    <t>CRN</t>
+  </si>
+  <si>
+    <t>Disposal_or_Release_Date</t>
+  </si>
+  <si>
+    <t>Sentence_Type</t>
+  </si>
+  <si>
+    <t>SO_Registration_Date</t>
+  </si>
+  <si>
+    <t>ARMS1</t>
+  </si>
+  <si>
+    <t>Test Arms Assessment</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>C1234567</t>
+  </si>
+  <si>
+    <t>License</t>
+  </si>
+  <si>
+    <t>ARMS2</t>
+  </si>
+  <si>
+    <t>C1234568</t>
+  </si>
+  <si>
+    <t>GS1</t>
+  </si>
+  <si>
+    <t>Group supervision</t>
+  </si>
+  <si>
+    <t>Billy Jones</t>
+  </si>
+  <si>
+    <t>PO</t>
+  </si>
+  <si>
+    <t>JWMT</t>
+  </si>
+  <si>
+    <t>Jane Jones</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -415,8 +491,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -429,8 +511,20 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0B64A0"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8FBFC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -490,13 +584,102 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3877A6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3877A6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3877A6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA5A5B1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3877A6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3877A6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA5A5B1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3877A6"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFEBEBEB"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFEBEBEB"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFEBEBEB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFEBEBEB"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFEBEBEB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFEBEBEB"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFEBEBEB"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFEBEBEB"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -521,6 +704,34 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -803,7 +1014,7 @@
   <dimension ref="A1:AO3"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:XFD1"/>
+      <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1223,82 +1434,82 @@
   <dimension ref="A1:AO1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:AO1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:41" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y1" s="2" t="s">
@@ -1310,16 +1521,16 @@
       <c r="AA1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AD1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="2" t="s">
         <v>22</v>
       </c>
       <c r="AF1" s="2" t="s">
@@ -1331,26 +1542,155 @@
       <c r="AH1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AI1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AK1" s="2" t="s">
         <v>28</v>
       </c>
       <c r="AL1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AN1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AO1" s="2" t="s">
         <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:12" ht="37" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="17">
+        <v>42991</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="11">
+        <v>1002</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="J2" s="17">
+        <v>42991</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L2" s="17">
+        <v>42991</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="17">
+        <v>42991</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="11">
+        <v>1002</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="J3" s="17">
+        <v>42991</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" s="17">
+        <v>42991</v>
       </c>
     </row>
   </sheetData>
@@ -2059,13 +2399,17 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="A2" sqref="A2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="22.1640625" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
@@ -2096,6 +2440,64 @@
         <v>104</v>
       </c>
     </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="11">
+        <v>999</v>
+      </c>
+      <c r="B2" s="17">
+        <v>43033</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="11">
+        <v>1003</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="11">
+        <v>888</v>
+      </c>
+      <c r="B3" s="17">
+        <v>43033</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" s="11">
+        <v>1003</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
175: Update column headers in example files and update tests for court reports
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/WMT_Extract_sample.xlsx
+++ b/wmt_etl/tests/data/WMT_Extract_sample.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="133">
   <si>
     <t>Trust</t>
   </si>
@@ -433,13 +433,22 @@
   </si>
   <si>
     <t>Jane Jones</t>
+  </si>
+  <si>
+    <t>LDU_Desc</t>
+  </si>
+  <si>
+    <t>LDU_Code</t>
+  </si>
+  <si>
+    <t>Oral_reports</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -496,8 +505,13 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -522,8 +536,14 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF666699"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -672,13 +692,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFA2BD90"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFA2BD90"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFA2BD90"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA2BD90"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFA2BD90"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFA2BD90"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA2BD90"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -729,6 +777,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1559,9 +1619,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:AO3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1572,90 +1634,187 @@
     <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="H1" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="K1" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="F1" t="s">
+      <c r="M1" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="G1" t="s">
+      <c r="N1" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="H1" t="s">
+      <c r="O1" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="I1" t="s">
+      <c r="P1" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q1" s="24" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+      <c r="AJ1" s="25"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1" s="25"/>
+      <c r="AM1" s="25"/>
+      <c r="AN1" s="25"/>
+      <c r="AO1" s="25"/>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
         <v>37</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G2" t="s">
         <v>38</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H2" t="s">
         <v>39</v>
       </c>
-      <c r="D2">
+      <c r="I2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2">
         <v>1001</v>
       </c>
-      <c r="E2" t="s">
+      <c r="K2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" t="s">
         <v>49</v>
       </c>
-      <c r="F2">
-        <v>15</v>
-      </c>
-      <c r="G2">
+      <c r="M2">
         <v>5</v>
       </c>
-      <c r="H2">
-        <v>24</v>
-      </c>
-      <c r="I2" s="3">
+      <c r="N2">
+        <v>4</v>
+      </c>
+      <c r="O2">
+        <v>3</v>
+      </c>
+      <c r="P2">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="3">
         <v>42795.628472222219</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="AO2" s="3"/>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
         <v>37</v>
       </c>
-      <c r="B3" t="s">
+      <c r="G3" t="s">
         <v>38</v>
       </c>
-      <c r="C3" t="s">
+      <c r="H3" t="s">
         <v>42</v>
       </c>
-      <c r="D3">
+      <c r="I3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3">
         <v>1002</v>
       </c>
-      <c r="E3" t="s">
+      <c r="K3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" t="s">
         <v>50</v>
       </c>
-      <c r="F3">
-        <v>18</v>
-      </c>
-      <c r="G3">
-        <v>11</v>
-      </c>
-      <c r="H3">
-        <v>13</v>
-      </c>
-      <c r="I3" s="3">
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>5</v>
+      </c>
+      <c r="P3">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="3">
         <v>42795.628472222219</v>
       </c>
     </row>
@@ -2260,7 +2419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:I3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
408: Update unit tests and excel files for outstanding reports
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/WMT_Extract_sample.xlsx
+++ b/wmt_etl/tests/data/WMT_Extract_sample.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caoimheb/Desktop/Excel files /"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caoimheb/Documents/MOJ_WMT/repos/wmt-etl/wmt_etl/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="GS" sheetId="9" r:id="rId9"/>
     <sheet name="ARMS" sheetId="10" r:id="rId10"/>
     <sheet name="T2A" sheetId="11" r:id="rId11"/>
+    <sheet name="WMT_Extract_SA" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="136">
   <si>
     <t>Trust</t>
   </si>
@@ -443,6 +444,15 @@
   </si>
   <si>
     <t>Oral_reports</t>
+  </si>
+  <si>
+    <t>Disposal_Type_Desc</t>
+  </si>
+  <si>
+    <t>Disposal_Type_Code</t>
+  </si>
+  <si>
+    <t>Standalone_Order</t>
   </si>
 </sst>
 </file>
@@ -544,7 +554,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -721,13 +731,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFCCCCFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -790,6 +828,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1758,11 +1802,55 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
WMT0115 Updated Test Extract spreadsheet with suspended_lifers tab. Updated tests to account for the new tab
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/WMT_Extract_sample.xlsx
+++ b/wmt_etl/tests/data/WMT_Extract_sample.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caoimheb/Documents/MOJ_WMT/repos/wmt-etl/wmt_etl/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinfox/Documents/WMT/wmt-etl/wmt_etl/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310B3398-2EEE-FA4F-8353-27D5F46FC177}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -24,8 +25,9 @@
     <sheet name="ARMS" sheetId="10" r:id="rId10"/>
     <sheet name="T2A" sheetId="11" r:id="rId11"/>
     <sheet name="WMT_Extract_SA" sheetId="12" r:id="rId12"/>
+    <sheet name="Suspended_Lifers" sheetId="13" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="152">
   <si>
     <t>Trust</t>
   </si>
@@ -453,13 +455,77 @@
   </si>
   <si>
     <t>Assessment_Team_Key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Row_Type
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Case_Ref_No
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tier_Code
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team_Code
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OM_Grade_Code
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In_Custody
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register_Code
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register_Description
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register_Level
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register_Level_Description
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register_Category
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deregistration_Date
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register_Category_Description
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registration_Date
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Next_Review_Date
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -765,7 +831,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -836,6 +902,9 @@
     <xf numFmtId="49" fontId="8" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -847,6 +916,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1114,14 +1186,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO3"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
@@ -1153,7 +1225,7 @@
     <col min="41" max="41" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" ht="17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1278,7 +1350,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:41">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1403,7 +1475,7 @@
         <v>42795.628472222219</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:41">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1534,16 +1606,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="37" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="37">
       <c r="A1" s="12" t="s">
         <v>105</v>
       </c>
@@ -1581,7 +1653,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="17">
         <v>42991</v>
       </c>
@@ -1619,7 +1691,7 @@
         <v>42991</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" s="17">
         <v>42991</v>
       </c>
@@ -1663,16 +1735,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AO1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:AO1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:41" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" ht="17">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1803,16 +1875,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="26" t="s">
         <v>52</v>
       </c>
@@ -1839,6 +1911,88 @@
       </c>
       <c r="I1" s="27" t="s">
         <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8253A4BC-8A65-7A44-968B-FB4159B96388}">
+  <dimension ref="A1:Q1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" customWidth="1"/>
+    <col min="11" max="11" width="27.6640625" customWidth="1"/>
+    <col min="12" max="12" width="18.5" customWidth="1"/>
+    <col min="13" max="13" width="17.5" customWidth="1"/>
+    <col min="14" max="14" width="26.1640625" customWidth="1"/>
+    <col min="15" max="15" width="18.1640625" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="53">
+      <c r="A1" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="O1" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="P1" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q1" s="28" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1847,14 +2001,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AO3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
@@ -1863,7 +2017,7 @@
     <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -1940,7 +2094,7 @@
       <c r="AN1" s="25"/>
       <c r="AO1" s="25"/>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:41">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1994,7 +2148,7 @@
       </c>
       <c r="AO2" s="3"/>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:41">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -2053,14 +2207,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
@@ -2072,7 +2226,7 @@
     <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2098,7 +2252,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -2121,7 +2275,7 @@
         <v>42795.628472222219</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -2153,14 +2307,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
@@ -2171,7 +2325,7 @@
     <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="17">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -2194,7 +2348,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="4" t="s">
         <v>62</v>
       </c>
@@ -2217,7 +2371,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="4" t="s">
         <v>62</v>
       </c>
@@ -2246,16 +2400,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="17">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -2278,7 +2432,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="4" t="s">
         <v>58</v>
       </c>
@@ -2301,7 +2455,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="4" t="s">
         <v>58</v>
       </c>
@@ -2330,16 +2484,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="17">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -2362,7 +2516,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="4" t="s">
         <v>68</v>
       </c>
@@ -2385,7 +2539,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="6" t="s">
         <v>68</v>
       </c>
@@ -2414,16 +2568,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="17">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -2446,7 +2600,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="4" t="s">
         <v>69</v>
       </c>
@@ -2469,7 +2623,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="6" t="s">
         <v>69</v>
       </c>
@@ -2498,16 +2652,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:14" s="8" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="8" customFormat="1" ht="23.25" customHeight="1">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -2551,7 +2705,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" s="9">
         <v>123</v>
       </c>
@@ -2595,7 +2749,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3">
         <v>321</v>
       </c>
@@ -2645,20 +2799,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="8" max="8" width="22.1640625" customWidth="1"/>
     <col min="9" max="9" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="11" t="s">
         <v>100</v>
       </c>
@@ -2687,7 +2841,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="11">
         <v>999</v>
       </c>
@@ -2716,7 +2870,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="11">
         <v>888</v>
       </c>

</xml_diff>

<commit_message>
WMT0115: Adding wmt_extract_filtered to the list of expected worksheet tabs.
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/WMT_Extract_sample.xlsx
+++ b/wmt_etl/tests/data/WMT_Extract_sample.xlsx
@@ -1,31 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinfox/Documents/WMT/wmt-etl/wmt_etl/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310B3398-2EEE-FA4F-8353-27D5F46FC177}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EBBC3A-2315-0C47-8F23-52C4ABD93C3B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
-    <sheet name="Court_Reports" sheetId="2" r:id="rId2"/>
-    <sheet name="Inst_Reports" sheetId="3" r:id="rId3"/>
-    <sheet name="Flag_Warr_4_n" sheetId="4" r:id="rId4"/>
-    <sheet name="Flag_Upw" sheetId="5" r:id="rId5"/>
-    <sheet name="Flag_O_Due" sheetId="6" r:id="rId6"/>
-    <sheet name="Flag_Priority" sheetId="7" r:id="rId7"/>
-    <sheet name="CMS" sheetId="8" r:id="rId8"/>
-    <sheet name="GS" sheetId="9" r:id="rId9"/>
-    <sheet name="ARMS" sheetId="10" r:id="rId10"/>
-    <sheet name="T2A" sheetId="11" r:id="rId11"/>
-    <sheet name="WMT_Extract_SA" sheetId="12" r:id="rId12"/>
-    <sheet name="Suspended_Lifers" sheetId="13" r:id="rId13"/>
+    <sheet name="WMT_Extract_Filtered" sheetId="14" r:id="rId2"/>
+    <sheet name="Court_Reports" sheetId="2" r:id="rId3"/>
+    <sheet name="Inst_Reports" sheetId="3" r:id="rId4"/>
+    <sheet name="Flag_Warr_4_n" sheetId="4" r:id="rId5"/>
+    <sheet name="Flag_Upw" sheetId="5" r:id="rId6"/>
+    <sheet name="Flag_O_Due" sheetId="6" r:id="rId7"/>
+    <sheet name="Flag_Priority" sheetId="7" r:id="rId8"/>
+    <sheet name="CMS" sheetId="8" r:id="rId9"/>
+    <sheet name="GS" sheetId="9" r:id="rId10"/>
+    <sheet name="ARMS" sheetId="10" r:id="rId11"/>
+    <sheet name="T2A" sheetId="11" r:id="rId12"/>
+    <sheet name="WMT_Extract_SA" sheetId="12" r:id="rId13"/>
+    <sheet name="Suspended_Lifers" sheetId="13" r:id="rId14"/>
   </sheets>
   <calcPr calcId="150000"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="152">
   <si>
     <t>Trust</t>
   </si>
@@ -525,7 +526,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -537,16 +538,19 @@
       <sz val="13"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -568,6 +572,7 @@
       <sz val="9"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -581,11 +586,13 @@
       <sz val="9"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1189,11 +1196,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
@@ -1225,7 +1232,7 @@
     <col min="41" max="41" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="17">
+    <row r="1" spans="1:41" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1350,7 +1357,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:41">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1475,7 +1482,7 @@
         <v>42795.628472222219</v>
       </c>
     </row>
-    <row r="3" spans="1:41">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1606,6 +1613,112 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="22.1640625" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="11">
+        <v>999</v>
+      </c>
+      <c r="B2" s="17">
+        <v>43033</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="F2" s="11">
+        <v>1003</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="11">
+        <v>888</v>
+      </c>
+      <c r="B3" s="17">
+        <v>43033</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" s="11">
+        <v>1003</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -1613,9 +1726,9 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="37">
+    <row r="1" spans="1:12" ht="40" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>105</v>
       </c>
@@ -1653,7 +1766,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="17">
         <v>42991</v>
       </c>
@@ -1691,7 +1804,7 @@
         <v>42991</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="17">
         <v>42991</v>
       </c>
@@ -1734,7 +1847,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AO1"/>
   <sheetViews>
@@ -1742,9 +1855,9 @@
       <selection sqref="A1:AO1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:41" ht="17">
+    <row r="1" spans="1:41" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1874,7 +1987,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
@@ -1882,9 +1995,9 @@
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>52</v>
       </c>
@@ -1918,15 +2031,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8253A4BC-8A65-7A44-968B-FB4159B96388}">
   <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
@@ -1942,7 +2055,7 @@
     <col min="16" max="16" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="53">
+    <row r="1" spans="1:17" ht="27" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
         <v>136</v>
       </c>
@@ -2001,6 +2114,399 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E51862E-3F0C-9744-83DC-1E2B92404767}">
+  <dimension ref="A1:AO3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AF20" sqref="AF20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="41" max="41" width="15.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:41" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2">
+        <v>1001</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+      <c r="M2">
+        <v>20</v>
+      </c>
+      <c r="N2">
+        <v>30</v>
+      </c>
+      <c r="O2">
+        <v>40</v>
+      </c>
+      <c r="P2">
+        <v>50</v>
+      </c>
+      <c r="Q2">
+        <v>60</v>
+      </c>
+      <c r="R2">
+        <v>70</v>
+      </c>
+      <c r="S2">
+        <v>80</v>
+      </c>
+      <c r="T2">
+        <v>90</v>
+      </c>
+      <c r="U2">
+        <v>20</v>
+      </c>
+      <c r="V2">
+        <v>30</v>
+      </c>
+      <c r="W2">
+        <v>40</v>
+      </c>
+      <c r="X2">
+        <v>50</v>
+      </c>
+      <c r="Y2">
+        <v>60</v>
+      </c>
+      <c r="Z2">
+        <v>70</v>
+      </c>
+      <c r="AA2">
+        <v>80</v>
+      </c>
+      <c r="AB2">
+        <v>90</v>
+      </c>
+      <c r="AC2">
+        <v>10</v>
+      </c>
+      <c r="AD2">
+        <v>20</v>
+      </c>
+      <c r="AE2">
+        <v>30</v>
+      </c>
+      <c r="AF2">
+        <v>40</v>
+      </c>
+      <c r="AG2">
+        <v>50</v>
+      </c>
+      <c r="AH2">
+        <v>60</v>
+      </c>
+      <c r="AI2">
+        <v>70</v>
+      </c>
+      <c r="AJ2">
+        <v>80</v>
+      </c>
+      <c r="AK2">
+        <v>90</v>
+      </c>
+      <c r="AL2">
+        <v>100</v>
+      </c>
+      <c r="AM2">
+        <v>40</v>
+      </c>
+      <c r="AN2">
+        <v>60</v>
+      </c>
+      <c r="AO2" s="3">
+        <v>42795.628472222219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3">
+        <v>1002</v>
+      </c>
+      <c r="L3">
+        <v>10</v>
+      </c>
+      <c r="M3">
+        <v>20</v>
+      </c>
+      <c r="N3">
+        <v>30</v>
+      </c>
+      <c r="O3">
+        <v>40</v>
+      </c>
+      <c r="P3">
+        <v>50</v>
+      </c>
+      <c r="Q3">
+        <v>60</v>
+      </c>
+      <c r="R3">
+        <v>70</v>
+      </c>
+      <c r="S3">
+        <v>80</v>
+      </c>
+      <c r="T3">
+        <v>90</v>
+      </c>
+      <c r="U3">
+        <v>20</v>
+      </c>
+      <c r="V3">
+        <v>30</v>
+      </c>
+      <c r="W3">
+        <v>40</v>
+      </c>
+      <c r="X3">
+        <v>10</v>
+      </c>
+      <c r="Y3">
+        <v>20</v>
+      </c>
+      <c r="Z3">
+        <v>30</v>
+      </c>
+      <c r="AA3">
+        <v>40</v>
+      </c>
+      <c r="AB3">
+        <v>50</v>
+      </c>
+      <c r="AC3">
+        <v>60</v>
+      </c>
+      <c r="AD3">
+        <v>70</v>
+      </c>
+      <c r="AE3">
+        <v>80</v>
+      </c>
+      <c r="AF3">
+        <v>90</v>
+      </c>
+      <c r="AG3">
+        <v>50</v>
+      </c>
+      <c r="AH3">
+        <v>40</v>
+      </c>
+      <c r="AI3">
+        <v>20</v>
+      </c>
+      <c r="AJ3">
+        <v>20</v>
+      </c>
+      <c r="AK3">
+        <v>30</v>
+      </c>
+      <c r="AL3">
+        <v>50</v>
+      </c>
+      <c r="AM3">
+        <v>80</v>
+      </c>
+      <c r="AN3">
+        <v>90</v>
+      </c>
+      <c r="AO3" s="3">
+        <v>42795.628472222219</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AO3"/>
   <sheetViews>
@@ -2008,7 +2514,7 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
@@ -2017,7 +2523,7 @@
     <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -2094,7 +2600,7 @@
       <c r="AN1" s="25"/>
       <c r="AO1" s="25"/>
     </row>
-    <row r="2" spans="1:41">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -2148,7 +2654,7 @@
       </c>
       <c r="AO2" s="3"/>
     </row>
-    <row r="3" spans="1:41">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -2206,7 +2712,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -2214,7 +2720,7 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
@@ -2226,7 +2732,7 @@
     <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2252,7 +2758,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -2275,7 +2781,7 @@
         <v>42795.628472222219</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -2306,7 +2812,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -2314,7 +2820,7 @@
       <selection activeCell="A2" sqref="A2:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
@@ -2325,7 +2831,7 @@
     <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17">
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -2348,7 +2854,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>62</v>
       </c>
@@ -2371,7 +2877,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>62</v>
       </c>
@@ -2399,7 +2905,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -2407,9 +2913,9 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="17">
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -2432,7 +2938,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>58</v>
       </c>
@@ -2455,7 +2961,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>58</v>
       </c>
@@ -2483,7 +2989,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -2491,9 +2997,9 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="17">
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -2516,7 +3022,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>68</v>
       </c>
@@ -2539,7 +3045,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>68</v>
       </c>
@@ -2567,7 +3073,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -2575,9 +3081,9 @@
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="17">
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -2600,7 +3106,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>69</v>
       </c>
@@ -2623,7 +3129,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>69</v>
       </c>
@@ -2651,7 +3157,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
@@ -2659,9 +3165,9 @@
       <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" s="8" customFormat="1" ht="23.25" customHeight="1">
+    <row r="1" spans="1:14" s="8" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -2705,7 +3211,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="9">
         <v>123</v>
       </c>
@@ -2749,7 +3255,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>321</v>
       </c>
@@ -2790,112 +3296,6 @@
         <v>38</v>
       </c>
       <c r="N3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:I3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="8" max="8" width="22.1640625" customWidth="1"/>
-    <col min="9" max="9" width="17.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="11">
-        <v>999</v>
-      </c>
-      <c r="B2" s="17">
-        <v>43033</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="F2" s="11">
-        <v>1003</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="11">
-        <v>888</v>
-      </c>
-      <c r="B3" s="17">
-        <v>43033</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="F3" s="11">
-        <v>1003</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="I3" s="11" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>